<commit_message>
Joins & AS command
</commit_message>
<xml_diff>
--- a/Excel/Práctica/14. BuscarV & BuscarH/FuncionBuscarV.xlsx
+++ b/Excel/Práctica/14. BuscarV & BuscarH/FuncionBuscarV.xlsx
@@ -2241,9 +2241,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2252,6 +2249,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2576,7 +2576,7 @@
   <dimension ref="A1:Q196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2610,12 +2610,12 @@
         <v>269</v>
       </c>
       <c r="F1"/>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2668,7 +2668,7 @@
         <v>407</v>
       </c>
       <c r="H3" t="str">
-        <f>VLOOKUP(G3,A2:E193,2,FALSE)</f>
+        <f>VLOOKUP(G3,$A$2:$E$193,2,FALSE)</f>
         <v>JOSE</v>
       </c>
       <c r="I3" t="str">
@@ -2679,14 +2679,14 @@
         <f>VLOOKUP(G3,A$2:E$193,4,FALSE)</f>
         <v>1500</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="15" t="s">
         <v>475</v>
       </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
     </row>
     <row r="4" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2709,7 +2709,7 @@
         <v>309</v>
       </c>
       <c r="H4" t="str">
-        <f>VLOOKUP(G4,A2:E193,2,FALSE)</f>
+        <f t="shared" ref="H4:H5" si="0">VLOOKUP(G4,$A$2:$E$193,2,FALSE)</f>
         <v>ANTONIO</v>
       </c>
       <c r="I4" t="str">
@@ -2720,12 +2720,12 @@
         <f>VLOOKUP(G4,A$2:E$193,4,FALSE)</f>
         <v>1500</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
     </row>
     <row r="5" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -2748,7 +2748,7 @@
         <v>461</v>
       </c>
       <c r="H5" t="str">
-        <f>VLOOKUP(G5,A3:E194,2,FALSE)</f>
+        <f>VLOOKUP(G5,$A$2:$E$193,2,FALSE)</f>
         <v>DAVID</v>
       </c>
       <c r="I5" t="str">
@@ -2759,12 +2759,12 @@
         <f>VLOOKUP(G5,A$2:E$193,4,FALSE)</f>
         <v>1100</v>
       </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
     </row>
     <row r="6" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -2783,12 +2783,12 @@
         <v>372</v>
       </c>
       <c r="F6"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
     </row>
     <row r="7" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2808,12 +2808,12 @@
       </c>
       <c r="F7"/>
       <c r="H7" s="10"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
     </row>
     <row r="8" spans="1:17" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -2832,18 +2832,18 @@
         <v>372</v>
       </c>
       <c r="F8"/>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="15" t="s">
         <v>474</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
     </row>
     <row r="9" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -2862,16 +2862,16 @@
         <v>272</v>
       </c>
       <c r="F9"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -2890,16 +2890,16 @@
         <v>271</v>
       </c>
       <c r="F10"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
     </row>
     <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2918,10 +2918,10 @@
         <v>272</v>
       </c>
       <c r="F11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:17" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2940,18 +2940,18 @@
         <v>372</v>
       </c>
       <c r="F12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="L12" s="12" t="s">
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="L12" s="15" t="s">
         <v>473</v>
       </c>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -2970,16 +2970,16 @@
         <v>272</v>
       </c>
       <c r="F13"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -2998,16 +2998,16 @@
         <v>270</v>
       </c>
       <c r="F14"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
     </row>
     <row r="15" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -3026,16 +3026,16 @@
         <v>272</v>
       </c>
       <c r="F15"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
     </row>
     <row r="16" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -3054,16 +3054,16 @@
         <v>372</v>
       </c>
       <c r="F16"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
     </row>
     <row r="17" spans="1:17" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -3082,16 +3082,16 @@
         <v>271</v>
       </c>
       <c r="F17"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
     </row>
     <row r="18" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -3110,16 +3110,16 @@
         <v>271</v>
       </c>
       <c r="F18"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
     </row>
     <row r="19" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -3138,10 +3138,10 @@
         <v>372</v>
       </c>
       <c r="F19"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -3160,18 +3160,18 @@
         <v>272</v>
       </c>
       <c r="F20"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="L20" s="12" t="s">
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="L20" s="15" t="s">
         <v>472</v>
       </c>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
     </row>
     <row r="21" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -3190,16 +3190,16 @@
         <v>372</v>
       </c>
       <c r="F21"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
     </row>
     <row r="22" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -3222,12 +3222,12 @@
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
     </row>
     <row r="23" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -3250,12 +3250,12 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
     </row>
     <row r="24" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -3278,12 +3278,12 @@
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
     </row>
     <row r="25" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -3302,12 +3302,12 @@
         <v>270</v>
       </c>
       <c r="F25"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
     </row>
     <row r="26" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -3326,12 +3326,12 @@
         <v>270</v>
       </c>
       <c r="F26"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
     </row>
     <row r="27" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -3368,14 +3368,14 @@
         <v>272</v>
       </c>
       <c r="F28"/>
-      <c r="L28" s="13" t="s">
+      <c r="L28" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
     </row>
     <row r="29" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -3394,12 +3394,12 @@
         <v>372</v>
       </c>
       <c r="F29"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
     </row>
     <row r="30" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -3436,14 +3436,14 @@
         <v>271</v>
       </c>
       <c r="F31"/>
-      <c r="L31" s="14" t="s">
+      <c r="L31" s="13" t="s">
         <v>471</v>
       </c>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
     </row>
     <row r="32" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -3462,12 +3462,12 @@
         <v>270</v>
       </c>
       <c r="F32"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
     </row>
     <row r="33" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">

</xml_diff>